<commit_message>
process raw data into factor data
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XiaochenLin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XiaochenLin\Desktop\Quantitative-Country-ETF-Trading-Strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F056CFE-BC60-4234-83F1-97F1D30854A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6B38DD-0274-413E-9C67-FF4273C09FC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="356">
   <si>
     <t>Ticker</t>
   </si>
@@ -593,6 +593,513 @@
   </si>
   <si>
     <t>Emerging</t>
+  </si>
+  <si>
+    <t>REER</t>
+  </si>
+  <si>
+    <t>BISBDKR Index</t>
+  </si>
+  <si>
+    <t>BISBFIR Index</t>
+  </si>
+  <si>
+    <t>BISBFRR Index</t>
+  </si>
+  <si>
+    <t>BISBDER Index</t>
+  </si>
+  <si>
+    <t>BISBGRR Index</t>
+  </si>
+  <si>
+    <t>BISBHKR Index</t>
+  </si>
+  <si>
+    <t>BISBINR Index</t>
+  </si>
+  <si>
+    <t>BISBIDR Index</t>
+  </si>
+  <si>
+    <t>BISBIER Index</t>
+  </si>
+  <si>
+    <t>BISBILR Index</t>
+  </si>
+  <si>
+    <t>BISBITR Index</t>
+  </si>
+  <si>
+    <t>BISBJPR Index</t>
+  </si>
+  <si>
+    <t>BISBKRR Index</t>
+  </si>
+  <si>
+    <t>BISBMYR Index</t>
+  </si>
+  <si>
+    <t>BISBMXR Index</t>
+  </si>
+  <si>
+    <t>BISBNLR Index</t>
+  </si>
+  <si>
+    <t>BISBNZR Index</t>
+  </si>
+  <si>
+    <t>BISBNOR Index</t>
+  </si>
+  <si>
+    <t>BISBPER Index</t>
+  </si>
+  <si>
+    <t>BISBPHR Index</t>
+  </si>
+  <si>
+    <t>BISBPLR Index</t>
+  </si>
+  <si>
+    <t>BISBPTR Index</t>
+  </si>
+  <si>
+    <t>BISBRUR Index</t>
+  </si>
+  <si>
+    <t>BISBSAR Index</t>
+  </si>
+  <si>
+    <t>BISBSGR Index</t>
+  </si>
+  <si>
+    <t>BISBBRR Index</t>
+  </si>
+  <si>
+    <t>BISBESR Index</t>
+  </si>
+  <si>
+    <t>BISBSER Index</t>
+  </si>
+  <si>
+    <t>BISBCHR Index</t>
+  </si>
+  <si>
+    <t>BISBTWR Index</t>
+  </si>
+  <si>
+    <t>BRERTH Index</t>
+  </si>
+  <si>
+    <t>BISBTRR Index</t>
+  </si>
+  <si>
+    <t>BISBAED Index</t>
+  </si>
+  <si>
+    <t>BISBGBR Index</t>
+  </si>
+  <si>
+    <t>BISBUSR Index</t>
+  </si>
+  <si>
+    <t>BISBARR Index</t>
+  </si>
+  <si>
+    <t>BISBAUR Index</t>
+  </si>
+  <si>
+    <t>BISBATR Index</t>
+  </si>
+  <si>
+    <t>BISBBER Index</t>
+  </si>
+  <si>
+    <t>BISBCAR Index</t>
+  </si>
+  <si>
+    <t>BISBCLR Index</t>
+  </si>
+  <si>
+    <t>BISBCNR Index</t>
+  </si>
+  <si>
+    <t>BISBCOP Index</t>
+  </si>
+  <si>
+    <t>GDDBARGE Index</t>
+  </si>
+  <si>
+    <t>GDDBAUSL Index</t>
+  </si>
+  <si>
+    <t>GDDBAUST Index</t>
+  </si>
+  <si>
+    <t>GDDBBELG Index</t>
+  </si>
+  <si>
+    <t>GDDBBRAZ Index</t>
+  </si>
+  <si>
+    <t>GDDBCANA Index</t>
+  </si>
+  <si>
+    <t>GDDBCHIL Index</t>
+  </si>
+  <si>
+    <t>GDDBCHIN Index</t>
+  </si>
+  <si>
+    <t>GDDBCOLO Index</t>
+  </si>
+  <si>
+    <t>GDDBDNMK Index</t>
+  </si>
+  <si>
+    <t>GDDBEGYP Index</t>
+  </si>
+  <si>
+    <t>GDDBFINL Index</t>
+  </si>
+  <si>
+    <t>GDDBFRAN Index</t>
+  </si>
+  <si>
+    <t>GDDBGERM Index</t>
+  </si>
+  <si>
+    <t>GDDBGREE Index</t>
+  </si>
+  <si>
+    <t>GDDBHOKO Index</t>
+  </si>
+  <si>
+    <t>GDDBINDA Index</t>
+  </si>
+  <si>
+    <t>GDDBIDNS Index</t>
+  </si>
+  <si>
+    <t>GDDBIREL Index</t>
+  </si>
+  <si>
+    <t>GDDBISRL Index</t>
+  </si>
+  <si>
+    <t>GDDBITLY Index</t>
+  </si>
+  <si>
+    <t>GDDBJAPN Index</t>
+  </si>
+  <si>
+    <t>GDDBSOKO Index</t>
+  </si>
+  <si>
+    <t>GDDBMALY Index</t>
+  </si>
+  <si>
+    <t>GDDBMXCO Index</t>
+  </si>
+  <si>
+    <t>GDDBNETH Index</t>
+  </si>
+  <si>
+    <t>GDDBNWZD Index</t>
+  </si>
+  <si>
+    <t>GDDBNORW Index</t>
+  </si>
+  <si>
+    <t>GDDBPAKI Index</t>
+  </si>
+  <si>
+    <t>GDDBPERU Index</t>
+  </si>
+  <si>
+    <t>GDDBPHIL Index</t>
+  </si>
+  <si>
+    <t>GDDBPOLA Index</t>
+  </si>
+  <si>
+    <t>GDDBPORT Index</t>
+  </si>
+  <si>
+    <t>GDDBQATA Index</t>
+  </si>
+  <si>
+    <t>GDDBRUSS Index</t>
+  </si>
+  <si>
+    <t>GDDBSAAR Index</t>
+  </si>
+  <si>
+    <t>GDDBSING Index</t>
+  </si>
+  <si>
+    <t>GDDBSOAF Index</t>
+  </si>
+  <si>
+    <t>GDDBSPAN Index</t>
+  </si>
+  <si>
+    <t>GDDBSWED Index</t>
+  </si>
+  <si>
+    <t>GDDBSWIT Index</t>
+  </si>
+  <si>
+    <t>GDDBTIWN Index</t>
+  </si>
+  <si>
+    <t>GDDBTHAI Index</t>
+  </si>
+  <si>
+    <t>GDDBTURK Index</t>
+  </si>
+  <si>
+    <t>GDDBUNAE Index</t>
+  </si>
+  <si>
+    <t>GDDBUNKI Index</t>
+  </si>
+  <si>
+    <t>GDDBUNST Index</t>
+  </si>
+  <si>
+    <t>GDP Growth</t>
+  </si>
+  <si>
+    <t>Debt/GDP</t>
+  </si>
+  <si>
+    <t>ECGDAR 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDAU 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDAT 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDBE 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDBR 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDCA 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDCL 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDCN 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDCO 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDDK 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDEG 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDFI 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDFR 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDDE 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDGR 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDHK 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDIN 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDID 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDIE 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDIL 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDJP 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDKR 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDMY 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDMX 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDNL 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDNZ 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDNO 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDPK 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDPE 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDPH 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDPL 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDPT 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDQA 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDRU 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDSA 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDSG 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDZA 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDES 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDSE 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDCH 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDTW 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDTH 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDTR 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDAE 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDGB 20 Index</t>
+  </si>
+  <si>
+    <t>ECGDUS 20 Index</t>
+  </si>
+  <si>
+    <t>PMI</t>
+  </si>
+  <si>
+    <t>MPMIAUMA Index</t>
+  </si>
+  <si>
+    <t>MPMIATMA Index</t>
+  </si>
+  <si>
+    <t>MPMIBRMA Index</t>
+  </si>
+  <si>
+    <t>MPMICAMA Index</t>
+  </si>
+  <si>
+    <t>MPMICNMA Index</t>
+  </si>
+  <si>
+    <t>MPMICOMA Index</t>
+  </si>
+  <si>
+    <t>DEPMPMI Index</t>
+  </si>
+  <si>
+    <t>MPMIFRMA Index</t>
+  </si>
+  <si>
+    <t>MPMIDEMA Index</t>
+  </si>
+  <si>
+    <t>MPMIGRMA Index</t>
+  </si>
+  <si>
+    <t>MPMIHKWA Index</t>
+  </si>
+  <si>
+    <t>MPMIINMA Index</t>
+  </si>
+  <si>
+    <t>MPMIIDMA Index</t>
+  </si>
+  <si>
+    <t>MPMIIEMA Index</t>
+  </si>
+  <si>
+    <t>MPMIITMA Index</t>
+  </si>
+  <si>
+    <t>MPMIJPMA Index</t>
+  </si>
+  <si>
+    <t>MPMIKRMA Index</t>
+  </si>
+  <si>
+    <t>MPMIMYMA Index</t>
+  </si>
+  <si>
+    <t>MPMIMXMA Index</t>
+  </si>
+  <si>
+    <t>MPMINLMA Index</t>
+  </si>
+  <si>
+    <t>MPMIPHMA Index</t>
+  </si>
+  <si>
+    <t>MPMIPLMA Index</t>
+  </si>
+  <si>
+    <t>MPMIRUMA Index</t>
+  </si>
+  <si>
+    <t>MPMIESMA Index</t>
+  </si>
+  <si>
+    <t>MPMITWMA Index</t>
+  </si>
+  <si>
+    <t>MPMITHMA Index</t>
+  </si>
+  <si>
+    <t>MPMITRMA Index</t>
+  </si>
+  <si>
+    <t>MPMIGBMA Index</t>
+  </si>
+  <si>
+    <t>MPMIUSMA Index</t>
   </si>
 </sst>
 </file>
@@ -1407,20 +1914,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1428,16 +1941,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1445,16 +1970,25 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
         <v>145</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1462,16 +1996,28 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" t="s">
         <v>146</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1479,16 +2025,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" t="s">
         <v>147</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1496,16 +2054,25 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" t="s">
         <v>147</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1513,16 +2080,28 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" t="s">
         <v>148</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H6" t="s">
+        <v>284</v>
+      </c>
+      <c r="I6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1530,16 +2109,28 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="s">
         <v>149</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>227</v>
+      </c>
+      <c r="G7" t="s">
+        <v>236</v>
+      </c>
+      <c r="H7" t="s">
+        <v>285</v>
+      </c>
+      <c r="I7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1547,16 +2138,25 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" t="s">
         <v>150</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>228</v>
+      </c>
+      <c r="G8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1564,16 +2164,28 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" t="s">
         <v>151</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G9" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" t="s">
+        <v>287</v>
+      </c>
+      <c r="I9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1581,16 +2193,28 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" t="s">
         <v>152</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H10" t="s">
+        <v>288</v>
+      </c>
+      <c r="I10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1598,16 +2222,28 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" t="s">
         <v>153</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" t="s">
+        <v>240</v>
+      </c>
+      <c r="H11" t="s">
+        <v>289</v>
+      </c>
+      <c r="I11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1615,16 +2251,22 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" t="s">
         <v>154</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>241</v>
+      </c>
+      <c r="H12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1632,16 +2274,25 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" t="s">
         <v>147</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" t="s">
+        <v>242</v>
+      </c>
+      <c r="H13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1649,16 +2300,28 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" t="s">
         <v>147</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" t="s">
+        <v>243</v>
+      </c>
+      <c r="H14" t="s">
+        <v>292</v>
+      </c>
+      <c r="I14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1666,16 +2329,28 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" t="s">
         <v>147</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" t="s">
+        <v>244</v>
+      </c>
+      <c r="H15" t="s">
+        <v>293</v>
+      </c>
+      <c r="I15" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1683,16 +2358,28 @@
         <v>47</v>
       </c>
       <c r="C16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" t="s">
         <v>147</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" t="s">
+        <v>245</v>
+      </c>
+      <c r="H16" t="s">
+        <v>294</v>
+      </c>
+      <c r="I16" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1700,16 +2387,28 @@
         <v>50</v>
       </c>
       <c r="C17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" t="s">
         <v>155</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" t="s">
+        <v>246</v>
+      </c>
+      <c r="H17" t="s">
+        <v>295</v>
+      </c>
+      <c r="I17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1717,16 +2416,28 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" t="s">
         <v>156</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>194</v>
+      </c>
+      <c r="G18" t="s">
+        <v>247</v>
+      </c>
+      <c r="H18" t="s">
+        <v>296</v>
+      </c>
+      <c r="I18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1734,16 +2445,28 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" t="s">
         <v>157</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>57</v>
       </c>
-      <c r="E19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G19" t="s">
+        <v>248</v>
+      </c>
+      <c r="H19" t="s">
+        <v>297</v>
+      </c>
+      <c r="I19" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1751,16 +2474,28 @@
         <v>59</v>
       </c>
       <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" t="s">
         <v>147</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>60</v>
       </c>
-      <c r="E20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" t="s">
+        <v>249</v>
+      </c>
+      <c r="H20" t="s">
+        <v>298</v>
+      </c>
+      <c r="I20" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1768,16 +2503,25 @@
         <v>62</v>
       </c>
       <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" t="s">
         <v>158</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>63</v>
       </c>
-      <c r="E21" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" t="s">
+        <v>250</v>
+      </c>
+      <c r="H21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1785,16 +2529,25 @@
         <v>65</v>
       </c>
       <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" t="s">
         <v>147</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>66</v>
       </c>
-      <c r="E22" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" t="s">
+        <v>251</v>
+      </c>
+      <c r="I22" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1802,16 +2555,28 @@
         <v>68</v>
       </c>
       <c r="C23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" t="s">
         <v>159</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>69</v>
       </c>
-      <c r="E23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G23" t="s">
+        <v>252</v>
+      </c>
+      <c r="H23" t="s">
+        <v>300</v>
+      </c>
+      <c r="I23" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -1819,16 +2584,28 @@
         <v>71</v>
       </c>
       <c r="C24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" t="s">
         <v>160</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>72</v>
       </c>
-      <c r="E24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G24" t="s">
+        <v>253</v>
+      </c>
+      <c r="H24" t="s">
+        <v>301</v>
+      </c>
+      <c r="I24" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -1836,16 +2613,28 @@
         <v>74</v>
       </c>
       <c r="C25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" t="s">
         <v>161</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>75</v>
       </c>
-      <c r="E25" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" t="s">
+        <v>254</v>
+      </c>
+      <c r="H25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I25" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1853,16 +2642,28 @@
         <v>77</v>
       </c>
       <c r="C26" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" t="s">
         <v>162</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G26" t="s">
+        <v>255</v>
+      </c>
+      <c r="H26" t="s">
+        <v>303</v>
+      </c>
+      <c r="I26" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1870,16 +2671,28 @@
         <v>80</v>
       </c>
       <c r="C27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" t="s">
         <v>147</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>81</v>
       </c>
-      <c r="E27" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>203</v>
+      </c>
+      <c r="G27" t="s">
+        <v>256</v>
+      </c>
+      <c r="H27" t="s">
+        <v>304</v>
+      </c>
+      <c r="I27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1887,16 +2700,25 @@
         <v>83</v>
       </c>
       <c r="C28" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" t="s">
         <v>163</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>84</v>
       </c>
-      <c r="E28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>204</v>
+      </c>
+      <c r="G28" t="s">
+        <v>257</v>
+      </c>
+      <c r="H28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1904,16 +2726,25 @@
         <v>86</v>
       </c>
       <c r="C29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" t="s">
         <v>164</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>87</v>
       </c>
-      <c r="E29" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" t="s">
+        <v>258</v>
+      </c>
+      <c r="H29" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1921,16 +2752,22 @@
         <v>89</v>
       </c>
       <c r="C30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" t="s">
         <v>165</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>90</v>
       </c>
-      <c r="E30" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>259</v>
+      </c>
+      <c r="H30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -1938,16 +2775,25 @@
         <v>92</v>
       </c>
       <c r="C31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" t="s">
         <v>166</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>93</v>
       </c>
-      <c r="E31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>206</v>
+      </c>
+      <c r="G31" t="s">
+        <v>260</v>
+      </c>
+      <c r="H31" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -1955,16 +2801,28 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" t="s">
         <v>167</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>96</v>
       </c>
-      <c r="E32" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" t="s">
+        <v>261</v>
+      </c>
+      <c r="H32" t="s">
+        <v>309</v>
+      </c>
+      <c r="I32" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -1972,16 +2830,28 @@
         <v>98</v>
       </c>
       <c r="C33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" t="s">
         <v>168</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>99</v>
       </c>
-      <c r="E33" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" t="s">
+        <v>262</v>
+      </c>
+      <c r="H33" t="s">
+        <v>310</v>
+      </c>
+      <c r="I33" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1989,16 +2859,25 @@
         <v>101</v>
       </c>
       <c r="C34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" t="s">
         <v>147</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>102</v>
       </c>
-      <c r="E34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>209</v>
+      </c>
+      <c r="G34" t="s">
+        <v>263</v>
+      </c>
+      <c r="H34" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2006,16 +2885,22 @@
         <v>104</v>
       </c>
       <c r="C35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" t="s">
         <v>169</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>105</v>
       </c>
-      <c r="E35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>264</v>
+      </c>
+      <c r="H35" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -2023,16 +2908,28 @@
         <v>107</v>
       </c>
       <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" t="s">
         <v>170</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>108</v>
       </c>
-      <c r="E36" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>210</v>
+      </c>
+      <c r="G36" t="s">
+        <v>265</v>
+      </c>
+      <c r="H36" t="s">
+        <v>313</v>
+      </c>
+      <c r="I36" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -2040,16 +2937,25 @@
         <v>110</v>
       </c>
       <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
         <v>171</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>111</v>
       </c>
-      <c r="E37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>211</v>
+      </c>
+      <c r="G37" t="s">
+        <v>266</v>
+      </c>
+      <c r="H37" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -2057,16 +2963,25 @@
         <v>113</v>
       </c>
       <c r="C38" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" t="s">
         <v>172</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>114</v>
       </c>
-      <c r="E38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>212</v>
+      </c>
+      <c r="G38" t="s">
+        <v>267</v>
+      </c>
+      <c r="H38" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -2074,16 +2989,22 @@
         <v>116</v>
       </c>
       <c r="C39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" t="s">
         <v>173</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>117</v>
       </c>
-      <c r="E39" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>268</v>
+      </c>
+      <c r="H39" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -2091,16 +3012,28 @@
         <v>119</v>
       </c>
       <c r="C40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" t="s">
         <v>147</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>120</v>
       </c>
-      <c r="E40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>214</v>
+      </c>
+      <c r="G40" t="s">
+        <v>269</v>
+      </c>
+      <c r="H40" t="s">
+        <v>317</v>
+      </c>
+      <c r="I40" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -2108,16 +3041,25 @@
         <v>122</v>
       </c>
       <c r="C41" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" t="s">
         <v>174</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>123</v>
       </c>
-      <c r="E41" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>215</v>
+      </c>
+      <c r="G41" t="s">
+        <v>270</v>
+      </c>
+      <c r="H41" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -2125,16 +3067,25 @@
         <v>125</v>
       </c>
       <c r="C42" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" t="s">
         <v>175</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>126</v>
       </c>
-      <c r="E42" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>216</v>
+      </c>
+      <c r="G42" t="s">
+        <v>271</v>
+      </c>
+      <c r="H42" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -2142,16 +3093,28 @@
         <v>128</v>
       </c>
       <c r="C43" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43" t="s">
         <v>176</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>129</v>
       </c>
-      <c r="E43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>217</v>
+      </c>
+      <c r="G43" t="s">
+        <v>272</v>
+      </c>
+      <c r="H43" t="s">
+        <v>320</v>
+      </c>
+      <c r="I43" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>130</v>
       </c>
@@ -2159,16 +3122,28 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" t="s">
         <v>177</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>132</v>
       </c>
-      <c r="E44" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>218</v>
+      </c>
+      <c r="G44" t="s">
+        <v>273</v>
+      </c>
+      <c r="H44" t="s">
+        <v>321</v>
+      </c>
+      <c r="I44" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -2176,16 +3151,28 @@
         <v>134</v>
       </c>
       <c r="C45" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" t="s">
         <v>178</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>135</v>
       </c>
-      <c r="E45" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>219</v>
+      </c>
+      <c r="G45" t="s">
+        <v>274</v>
+      </c>
+      <c r="H45" t="s">
+        <v>322</v>
+      </c>
+      <c r="I45" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -2193,16 +3180,25 @@
         <v>137</v>
       </c>
       <c r="C46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" t="s">
         <v>179</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>138</v>
       </c>
-      <c r="E46" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>220</v>
+      </c>
+      <c r="G46" t="s">
+        <v>275</v>
+      </c>
+      <c r="H46" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -2210,16 +3206,28 @@
         <v>140</v>
       </c>
       <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" t="s">
         <v>180</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>141</v>
       </c>
-      <c r="E47" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>221</v>
+      </c>
+      <c r="G47" t="s">
+        <v>276</v>
+      </c>
+      <c r="H47" t="s">
+        <v>324</v>
+      </c>
+      <c r="I47" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -2227,13 +3235,25 @@
         <v>143</v>
       </c>
       <c r="C48" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" t="s">
         <v>181</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>144</v>
       </c>
-      <c r="E48" t="s">
-        <v>185</v>
+      <c r="F48" t="s">
+        <v>222</v>
+      </c>
+      <c r="G48" t="s">
+        <v>277</v>
+      </c>
+      <c r="H48" t="s">
+        <v>325</v>
+      </c>
+      <c r="I48" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>